<commit_message>
Update data and plot theme.
</commit_message>
<xml_diff>
--- a/data/use-of-cultural-activities-dk-2019.xlsx
+++ b/data/use-of-cultural-activities-dk-2019.xlsx
@@ -16,37 +16,37 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
   <x:si>
-    <x:t>Forbrug af kulturaktiviteter (år) indenfor de seneste tre måneder efter tid, område og kulturaktivitet</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Enhed: Pct.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Har været i biografen</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Har været til rytmisk og/eller klassisk koncert</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Har opsøgt billedkunst</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Har læst eller lyttet til skønlitterære bøger</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Har læst eller lyttet til faglitterære bøger</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Har været (fysisk) på biblioteket</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Har brugt bibliotekets digitale tjenester</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Har besøgt et museum o. lign</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Har overværet scenekunst i teatret, operaen på teaterfestival eller i det offentlige rum</x:t>
+    <x:t>Individuals use of cultural activities (year) within the past three months by time, area and cultural activities</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Units: Per cent</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Have been to the cinema</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Have been to concert</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Have seen visual arts (on pupose)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Have read or listened to fiction</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Have read or listened to non-fiction</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Have visited the library (physical visit)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Have used the librarys digital services</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Visited a museum etc.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Have watched performing arts in theater, opera, festivals or in public spaces</x:t>
   </x:si>
   <x:si>
     <x:t>2019</x:t>
@@ -55,16 +55,16 @@
     <x:t>Region Hovedstaden</x:t>
   </x:si>
   <x:si>
-    <x:t>Landsdel Byen København</x:t>
-  </x:si>
-  <x:si>
-    <x:t>København</x:t>
+    <x:t>Province Byen København</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Copenhagen</x:t>
   </x:si>
   <x:si>
     <x:t>Frederiksberg</x:t>
   </x:si>
   <x:si>
-    <x:t>Landsdel Københavns omegn</x:t>
+    <x:t>Province Københavns omegn</x:t>
   </x:si>
   <x:si>
     <x:t>Gentofte</x:t>
@@ -73,7 +73,7 @@
     <x:t>Gladsaxe</x:t>
   </x:si>
   <x:si>
-    <x:t>Landsdel Nordsjælland</x:t>
+    <x:t>Province Nordsjælland</x:t>
   </x:si>
   <x:si>
     <x:t>Egedal</x:t>
@@ -88,13 +88,13 @@
     <x:t>Rudersdal</x:t>
   </x:si>
   <x:si>
-    <x:t>Landsdel Bornholm</x:t>
+    <x:t>Province Bornholm</x:t>
   </x:si>
   <x:si>
     <x:t>Region Sjælland</x:t>
   </x:si>
   <x:si>
-    <x:t>Landsdel Østsjælland</x:t>
+    <x:t>Province Østsjælland</x:t>
   </x:si>
   <x:si>
     <x:t>Greve</x:t>
@@ -106,7 +106,7 @@
     <x:t>Roskilde</x:t>
   </x:si>
   <x:si>
-    <x:t>Landsdel Vest- og Sydsjælland</x:t>
+    <x:t>Province Vest- og Sydsjælland</x:t>
   </x:si>
   <x:si>
     <x:t>Guldborgsund</x:t>
@@ -127,7 +127,7 @@
     <x:t>Region Syddanmark</x:t>
   </x:si>
   <x:si>
-    <x:t>Landsdel Fyn</x:t>
+    <x:t>Province Fyn</x:t>
   </x:si>
   <x:si>
     <x:t>Assens</x:t>
@@ -142,7 +142,7 @@
     <x:t>Svendborg</x:t>
   </x:si>
   <x:si>
-    <x:t>Landsdel Sydjylland</x:t>
+    <x:t>Province Sydjylland</x:t>
   </x:si>
   <x:si>
     <x:t>Esbjerg</x:t>
@@ -172,7 +172,7 @@
     <x:t>Region Midtjylland</x:t>
   </x:si>
   <x:si>
-    <x:t>Landsdel Østjylland</x:t>
+    <x:t>Province Østjylland</x:t>
   </x:si>
   <x:si>
     <x:t>Favrskov</x:t>
@@ -196,7 +196,7 @@
     <x:t>Aarhus</x:t>
   </x:si>
   <x:si>
-    <x:t>Landsdel Vestjylland</x:t>
+    <x:t>Province Vestjylland</x:t>
   </x:si>
   <x:si>
     <x:t>Herning</x:t>
@@ -217,7 +217,7 @@
     <x:t>Region Nordjylland</x:t>
   </x:si>
   <x:si>
-    <x:t>Landsdel Nordjylland</x:t>
+    <x:t>Province Nordjylland</x:t>
   </x:si>
   <x:si>
     <x:t>Frederikshavn</x:t>
@@ -232,7 +232,7 @@
     <x:t>Aalborg</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">Film og serier er enten set derhjemme eller uden for hjemmet fx på farten og 'Har været i biografen'. Musik er hørt under transport, derhjemme og/eller ude i byen og omfatter 'Har været til rytmisk og/eller klassisk koncert'. 'Har overværet eller lyttet til en sportsbegivenhed' er sport set derhjemme og/eller i byen, og omfatter 'Har været til sportsbegivenhed som tilskuer. 2018 dækker juli 2018-juni 2019. 2019 dækker juli 2019-juni 2020. Diskretionerede kommun </x:t>
+    <x:t xml:space="preserve">'Have seen movies and series' covers watching at home or outside and includes 'Have been in the cinema'. 'Have listened to music' is music at home or out of home and includes 'Have been to a concert'. 'Have watched or listened to a sporting event' is sport watched at home eg on television and/or in the city, and includes the activity 'Been to a sport event as a spectator'. Discretioniced municipalities and Bornholm have few observations </x:t>
   </x:si>
 </x:sst>
 </file>
@@ -649,15 +649,15 @@
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
     <x:col min="1" max="1" width="40.710625" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="28.700625" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="21.700625" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="40.710625" style="0" customWidth="1"/>
-    <x:col min="5" max="5" width="22.840625" style="0" customWidth="1"/>
-    <x:col min="6" max="6" width="40.550625000000004" style="0" customWidth="1"/>
-    <x:col min="7" max="7" width="39.130625" style="0" customWidth="1"/>
-    <x:col min="8" max="8" width="31.410625" style="0" customWidth="1"/>
-    <x:col min="9" max="9" width="37.980625" style="0" customWidth="1"/>
-    <x:col min="10" max="10" width="28.700625" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="28.550625" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="24.980625" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="21.700625" style="0" customWidth="1"/>
+    <x:col min="5" max="5" width="32.550625" style="0" customWidth="1"/>
+    <x:col min="6" max="6" width="30.130625000000002" style="0" customWidth="1"/>
+    <x:col min="7" max="7" width="34.270625" style="0" customWidth="1"/>
+    <x:col min="8" max="8" width="36.550625000000004" style="0" customWidth="1"/>
+    <x:col min="9" max="9" width="36.130625" style="0" customWidth="1"/>
+    <x:col min="10" max="10" width="22.550625" style="0" customWidth="1"/>
     <x:col min="11" max="11" width="40.710625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>

</xml_diff>